<commit_message>
Remove quiz module and change IP logic for multiple people to use the same IP (bayreuth)
</commit_message>
<xml_diff>
--- a/userDataScripts/Usernames_Iceberg.xlsx
+++ b/userDataScripts/Usernames_Iceberg.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LocalAdmin\Nextcloud\MG\02_Arbeiten\Schuster_Richard_MA\CRUserManagement\userDataScripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LocalAdmin\Nextcloud\MG\05_SocCyberRange\userDataScripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB04A967-14FC-46B3-914A-543C6E174C5E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F90F5C-4FD6-4F29-8429-45253F56094A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Round1" sheetId="1" r:id="rId1"/>
     <sheet name="Round2" sheetId="2" r:id="rId2"/>
     <sheet name="Round3" sheetId="3" r:id="rId3"/>
     <sheet name="Round4" sheetId="4" r:id="rId4"/>
+    <sheet name="Round7" sheetId="5" r:id="rId5"/>
+    <sheet name="Round8" sheetId="6" r:id="rId6"/>
+    <sheet name="Round9" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="126">
   <si>
     <t>VirtualVeronica</t>
   </si>
@@ -307,6 +310,105 @@
   </si>
   <si>
     <t>HardwareHarry</t>
+  </si>
+  <si>
+    <t>LenzLena</t>
+  </si>
+  <si>
+    <t>BasilikumBasti</t>
+  </si>
+  <si>
+    <t>SonnenscheinStefan</t>
+  </si>
+  <si>
+    <t>FrühlingsFabi</t>
+  </si>
+  <si>
+    <t>LeberblümchenLudwig</t>
+  </si>
+  <si>
+    <t>ApfelblüteAlbert</t>
+  </si>
+  <si>
+    <t>DuftDaniel</t>
+  </si>
+  <si>
+    <t>GrünGloriya</t>
+  </si>
+  <si>
+    <t>VogelViktor</t>
+  </si>
+  <si>
+    <t>MaikäferManfred</t>
+  </si>
+  <si>
+    <t>FredFruchtig</t>
+  </si>
+  <si>
+    <t>FlanierFlo</t>
+  </si>
+  <si>
+    <t>SommerSebastian</t>
+  </si>
+  <si>
+    <t>KnospenKorbinian</t>
+  </si>
+  <si>
+    <t>SpargelSabrina</t>
+  </si>
+  <si>
+    <t>PusteblumenPhilip</t>
+  </si>
+  <si>
+    <t>HellHerbert</t>
+  </si>
+  <si>
+    <t>GezwitscherGeli</t>
+  </si>
+  <si>
+    <t>AprilwetterAndreas</t>
+  </si>
+  <si>
+    <t>BlütenBene</t>
+  </si>
+  <si>
+    <t>EisheiligenEsther</t>
+  </si>
+  <si>
+    <t>RadlRudi</t>
+  </si>
+  <si>
+    <t>PaprikaPetra</t>
+  </si>
+  <si>
+    <t>WeidenkätzchenWerner</t>
+  </si>
+  <si>
+    <t>SonnenscheinSascha</t>
+  </si>
+  <si>
+    <t>AperolAlex</t>
+  </si>
+  <si>
+    <t>ErdbeerEva</t>
+  </si>
+  <si>
+    <t>MarienkäferMichi</t>
+  </si>
+  <si>
+    <t>RosmarinRalf</t>
+  </si>
+  <si>
+    <t>BienenBernd</t>
+  </si>
+  <si>
+    <t>RosenRosa</t>
+  </si>
+  <si>
+    <t>WanderWolfgang</t>
+  </si>
+  <si>
+    <t>TauwetterTom</t>
   </si>
 </sst>
 </file>
@@ -633,13 +735,13 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -650,7 +752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>132199120101</v>
       </c>
@@ -661,7 +763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>132199120111</v>
       </c>
@@ -672,7 +774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>132199120117</v>
       </c>
@@ -683,7 +785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>132199120121</v>
       </c>
@@ -694,7 +796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>132199120133</v>
       </c>
@@ -705,7 +807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>132199120134</v>
       </c>
@@ -716,7 +818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>132199120144</v>
       </c>
@@ -727,7 +829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -738,7 +840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -749,7 +851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -760,7 +862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -771,7 +873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -782,7 +884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -793,7 +895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -804,7 +906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -815,7 +917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -826,7 +928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -837,7 +939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -848,7 +950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -868,17 +970,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D0108A0-FF41-4113-810C-43363852CDB6}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="3" width="27.140625" customWidth="1"/>
+    <col min="2" max="3" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -889,7 +991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>132199120101</v>
       </c>
@@ -900,7 +1002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>132199120111</v>
       </c>
@@ -911,7 +1013,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>132199120117</v>
       </c>
@@ -922,7 +1024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>132199120121</v>
       </c>
@@ -933,7 +1035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>132199120133</v>
       </c>
@@ -944,7 +1046,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>132199120134</v>
       </c>
@@ -955,7 +1057,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>132199120144</v>
       </c>
@@ -966,7 +1068,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -977,7 +1079,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -988,7 +1090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -999,7 +1101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1010,7 +1112,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1021,7 +1123,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1032,7 +1134,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1043,7 +1145,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1054,7 +1156,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1065,7 +1167,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1076,7 +1178,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1087,7 +1189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1108,16 +1210,16 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B17" sqref="B17:B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1128,7 +1230,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>132199120101</v>
       </c>
@@ -1139,7 +1241,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>132199120111</v>
       </c>
@@ -1150,7 +1252,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>132199120117</v>
       </c>
@@ -1161,7 +1263,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>132199120121</v>
       </c>
@@ -1172,7 +1274,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>132199120133</v>
       </c>
@@ -1183,7 +1285,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>132199120134</v>
       </c>
@@ -1194,7 +1296,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>132199120144</v>
       </c>
@@ -1205,7 +1307,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1216,7 +1318,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1227,7 +1329,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1238,7 +1340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1249,7 +1351,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1260,7 +1362,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1271,7 +1373,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1282,7 +1384,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1293,7 +1395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1304,7 +1406,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1315,7 +1417,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1326,7 +1428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1350,13 +1452,13 @@
       <selection activeCell="B1" sqref="B1:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1367,7 +1469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>132199120101</v>
       </c>
@@ -1378,7 +1480,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>132199120111</v>
       </c>
@@ -1389,7 +1491,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>132199120117</v>
       </c>
@@ -1400,7 +1502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>132199120121</v>
       </c>
@@ -1411,7 +1513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>132199120133</v>
       </c>
@@ -1422,7 +1524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>132199120134</v>
       </c>
@@ -1433,7 +1535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>132199120144</v>
       </c>
@@ -1444,7 +1546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1455,7 +1557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1466,7 +1568,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1477,7 +1579,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1488,7 +1590,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1499,7 +1601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1510,7 +1612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1521,7 +1623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1532,7 +1634,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1543,7 +1645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1554,7 +1656,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1565,7 +1667,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1574,6 +1676,242 @@
       </c>
       <c r="C20">
         <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F5AFF1-267C-4204-B289-3368D848351E}">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8B3F9B-DB48-47FE-8A7F-3D811DBCF3CD}">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CB9F857-9F0C-464F-A589-BB182A6253BD}">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated user management for team mode
</commit_message>
<xml_diff>
--- a/userDataScripts/Usernames_Iceberg.xlsx
+++ b/userDataScripts/Usernames_Iceberg.xlsx
@@ -1,26 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LocalAdmin\Nextcloud\MG\05_SocCyberRange\userDataScripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LocalAdmin\Nextcloud\MG\CRUserManagement_TeamMode\userDataScripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F90F5C-4FD6-4F29-8429-45253F56094A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF15712E-000E-44F2-A592-B195EF79CAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Round1" sheetId="1" r:id="rId1"/>
-    <sheet name="Round2" sheetId="2" r:id="rId2"/>
-    <sheet name="Round3" sheetId="3" r:id="rId3"/>
-    <sheet name="Round4" sheetId="4" r:id="rId4"/>
-    <sheet name="Round7" sheetId="5" r:id="rId5"/>
-    <sheet name="Round8" sheetId="6" r:id="rId6"/>
-    <sheet name="Round9" sheetId="7" r:id="rId7"/>
+    <sheet name="all" sheetId="8" r:id="rId1"/>
+    <sheet name="101" sheetId="9" r:id="rId2"/>
+    <sheet name="102" sheetId="11" r:id="rId3"/>
+    <sheet name="103" sheetId="10" r:id="rId4"/>
+    <sheet name="Round1" sheetId="1" r:id="rId5"/>
+    <sheet name="Round2" sheetId="2" r:id="rId6"/>
+    <sheet name="Round3" sheetId="3" r:id="rId7"/>
+    <sheet name="Round4" sheetId="4" r:id="rId8"/>
+    <sheet name="Round7" sheetId="5" r:id="rId9"/>
+    <sheet name="Round8" sheetId="6" r:id="rId10"/>
+    <sheet name="Round9" sheetId="7" r:id="rId11"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all!$A$1:$D$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="165">
   <si>
     <t>VirtualVeronica</t>
   </si>
@@ -409,13 +416,130 @@
   </si>
   <si>
     <t>TauwetterTom</t>
+  </si>
+  <si>
+    <t>CyberGuards</t>
+  </si>
+  <si>
+    <t>SafeCyberService</t>
+  </si>
+  <si>
+    <t>DemonicDataDefense</t>
+  </si>
+  <si>
+    <t>SystemSavers</t>
+  </si>
+  <si>
+    <t>EagleEyes</t>
+  </si>
+  <si>
+    <t>Cybermasters</t>
+  </si>
+  <si>
+    <t>SecurityAvengers</t>
+  </si>
+  <si>
+    <t>DataPatrol</t>
+  </si>
+  <si>
+    <t>GuardiansOfTheData</t>
+  </si>
+  <si>
+    <t>SecureWatchers</t>
+  </si>
+  <si>
+    <t>TheMasterminds</t>
+  </si>
+  <si>
+    <t>DefenseArt</t>
+  </si>
+  <si>
+    <t>ShieldAgainstAttacks</t>
+  </si>
+  <si>
+    <t>StayingOnAlert</t>
+  </si>
+  <si>
+    <t>GeniusesOnHold</t>
+  </si>
+  <si>
+    <t>UnbrokenDefense</t>
+  </si>
+  <si>
+    <t>ProtectiveShells</t>
+  </si>
+  <si>
+    <t>DataBreachDefenders</t>
+  </si>
+  <si>
+    <t>Cybernerds</t>
+  </si>
+  <si>
+    <t>MalwareAware</t>
+  </si>
+  <si>
+    <t>SOAREagles</t>
+  </si>
+  <si>
+    <t>RebootingRebels</t>
+  </si>
+  <si>
+    <t>NoToThreats</t>
+  </si>
+  <si>
+    <t>132.199.123.7</t>
+  </si>
+  <si>
+    <t>132.199.122.233</t>
+  </si>
+  <si>
+    <t>132.199.122.234</t>
+  </si>
+  <si>
+    <t>132.199.122.241</t>
+  </si>
+  <si>
+    <t>132.199.122.249</t>
+  </si>
+  <si>
+    <t>132.199.122.252</t>
+  </si>
+  <si>
+    <t>132.199.122.255</t>
+  </si>
+  <si>
+    <t>132.199.123.2</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>groupID</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>Backup1</t>
+  </si>
+  <si>
+    <t>Backup2</t>
+  </si>
+  <si>
+    <t>132.199.123.5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -423,16 +547,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -440,18 +578,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -728,6 +878,942 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE3895CD-0945-4EC3-943D-7F9E2870C570}">
+  <dimension ref="A1:E27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="2">
+        <v>101</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1830</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="2">
+        <v>101</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1039</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" s="2">
+        <v>101</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1492</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="2">
+        <v>101</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1239</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="2">
+        <v>101</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1673</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="2">
+        <v>101</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1928</v>
+      </c>
+      <c r="D7" s="2">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="2">
+        <v>101</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1849</v>
+      </c>
+      <c r="D8" s="2">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="3">
+        <v>101</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1450</v>
+      </c>
+      <c r="D9" s="3">
+        <v>8</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" s="2">
+        <v>102</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2295</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="2">
+        <v>102</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2840</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" s="2">
+        <v>102</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2767</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" s="2">
+        <v>102</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2691</v>
+      </c>
+      <c r="D13" s="2">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" s="2">
+        <v>102</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2489</v>
+      </c>
+      <c r="D14" s="2">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" s="2">
+        <v>102</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2944</v>
+      </c>
+      <c r="D15" s="2">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" s="2">
+        <v>102</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2812</v>
+      </c>
+      <c r="D16" s="2">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" s="3">
+        <v>102</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2091</v>
+      </c>
+      <c r="D17" s="3">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18">
+        <v>103</v>
+      </c>
+      <c r="C18">
+        <v>3991</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>145</v>
+      </c>
+      <c r="B19">
+        <v>103</v>
+      </c>
+      <c r="C19">
+        <v>3284</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20">
+        <v>103</v>
+      </c>
+      <c r="C20">
+        <v>3310</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>146</v>
+      </c>
+      <c r="B21">
+        <v>103</v>
+      </c>
+      <c r="C21">
+        <v>3849</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>147</v>
+      </c>
+      <c r="B22">
+        <v>103</v>
+      </c>
+      <c r="C22">
+        <v>3145</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23">
+        <v>103</v>
+      </c>
+      <c r="C23">
+        <v>3701</v>
+      </c>
+      <c r="D23">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>148</v>
+      </c>
+      <c r="B24">
+        <v>103</v>
+      </c>
+      <c r="C24">
+        <v>3656</v>
+      </c>
+      <c r="D24">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B25" s="3">
+        <v>103</v>
+      </c>
+      <c r="C25" s="3">
+        <v>3283</v>
+      </c>
+      <c r="D25" s="3">
+        <v>8</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>162</v>
+      </c>
+      <c r="E26" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>163</v>
+      </c>
+      <c r="E27" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D1" xr:uid="{FE3895CD-0945-4EC3-943D-7F9E2870C570}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8B3F9B-DB48-47FE-8A7F-3D811DBCF3CD}">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CB9F857-9F0C-464F-A589-BB182A6253BD}">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D9BEF8-8098-449A-ABCC-D1C9B0A4329C}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A397918-8305-4FAC-94A6-D87C9880E5B3}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{652E27E3-F811-4538-924D-4F6C0C94320C}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C7">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -735,13 +1821,13 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -752,7 +1838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>132199120101</v>
       </c>
@@ -763,7 +1849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>132199120111</v>
       </c>
@@ -774,7 +1860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>132199120117</v>
       </c>
@@ -785,7 +1871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>132199120121</v>
       </c>
@@ -796,7 +1882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>132199120133</v>
       </c>
@@ -807,7 +1893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>132199120134</v>
       </c>
@@ -818,7 +1904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>132199120144</v>
       </c>
@@ -829,7 +1915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -840,7 +1926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -851,7 +1937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -862,7 +1948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -873,7 +1959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -884,7 +1970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -895,7 +1981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -906,7 +1992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -917,7 +2003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -928,7 +2014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -939,7 +2025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -950,7 +2036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -966,7 +2052,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D0108A0-FF41-4113-810C-43363852CDB6}">
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -974,13 +2060,13 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="3" width="27.109375" customWidth="1"/>
+    <col min="2" max="3" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -991,7 +2077,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>132199120101</v>
       </c>
@@ -1002,7 +2088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>132199120111</v>
       </c>
@@ -1013,7 +2099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>132199120117</v>
       </c>
@@ -1024,7 +2110,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>132199120121</v>
       </c>
@@ -1035,7 +2121,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>132199120133</v>
       </c>
@@ -1046,7 +2132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>132199120134</v>
       </c>
@@ -1057,7 +2143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>132199120144</v>
       </c>
@@ -1068,7 +2154,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1079,7 +2165,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1090,7 +2176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1101,7 +2187,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1112,7 +2198,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1123,7 +2209,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1134,7 +2220,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1145,7 +2231,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1156,7 +2242,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1167,7 +2253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1178,7 +2264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1189,7 +2275,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1205,7 +2291,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57FDCF9F-E10C-4296-B991-3AD2517DC401}">
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -1213,13 +2299,13 @@
       <selection activeCell="B17" sqref="B17:B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1230,7 +2316,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>132199120101</v>
       </c>
@@ -1241,7 +2327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>132199120111</v>
       </c>
@@ -1252,7 +2338,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>132199120117</v>
       </c>
@@ -1263,7 +2349,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>132199120121</v>
       </c>
@@ -1274,7 +2360,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>132199120133</v>
       </c>
@@ -1285,7 +2371,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>132199120134</v>
       </c>
@@ -1296,7 +2382,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>132199120144</v>
       </c>
@@ -1307,7 +2393,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1318,7 +2404,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1329,7 +2415,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1340,7 +2426,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1351,7 +2437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1362,7 +2448,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1373,7 +2459,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1384,7 +2470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1395,7 +2481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1406,7 +2492,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1417,7 +2503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1428,7 +2514,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1444,7 +2530,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10704170-59C3-41D4-A18F-0E8E58D2DA07}">
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -1452,13 +2538,13 @@
       <selection activeCell="B1" sqref="B1:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1469,7 +2555,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>132199120101</v>
       </c>
@@ -1480,7 +2566,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>132199120111</v>
       </c>
@@ -1491,7 +2577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>132199120117</v>
       </c>
@@ -1502,7 +2588,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>132199120121</v>
       </c>
@@ -1513,7 +2599,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>132199120133</v>
       </c>
@@ -1524,7 +2610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>132199120134</v>
       </c>
@@ -1535,7 +2621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>132199120144</v>
       </c>
@@ -1546,7 +2632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1557,7 +2643,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1568,7 +2654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1579,7 +2665,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1590,7 +2676,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1601,7 +2687,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1612,7 +2698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1623,7 +2709,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1634,7 +2720,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1645,7 +2731,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1656,7 +2742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1667,7 +2753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1683,235 +2769,82 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F5AFF1-267C-4204-B289-3368D848351E}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.21875" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>105</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8B3F9B-DB48-47FE-8A7F-3D811DBCF3CD}">
-  <dimension ref="A1:A13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="29.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CB9F857-9F0C-464F-A589-BB182A6253BD}">
-  <dimension ref="A1:A11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>